<commit_message>
Update to summary for 2016-03-28
</commit_message>
<xml_diff>
--- a/results/2016-03-28/Summary.xlsx
+++ b/results/2016-03-28/Summary.xlsx
@@ -168,11 +168,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -2719,10 +2719,10 @@
     <tableColumn id="2" name="Committed"/>
     <tableColumn id="3" name="Private Bytes"/>
     <tableColumn id="4" name="Working Set"/>
-    <tableColumn id="9" name="Ratio vs Best (WS)" dataDxfId="1">
+    <tableColumn id="9" name="Ratio vs Best (WS)" dataDxfId="2">
       <calculatedColumnFormula>ROUND(AfterLoad[[#This Row],[Working Set]]/MIN(AfterLoad[Working Set]),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Ratio vs Best (PB)" dataDxfId="2">
+    <tableColumn id="6" name="Ratio vs Best (PB)" dataDxfId="1">
       <calculatedColumnFormula>ROUND(AfterLoad[[#This Row],[Private Bytes]]/MIN(AfterLoad[Private Bytes]),1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="Ratio vs Best (RPS)" dataDxfId="0">
@@ -3058,9 +3058,9 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3105,7 +3105,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
@@ -3149,7 +3149,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B6">
@@ -3193,7 +3193,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8">
@@ -3237,7 +3237,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B10">
@@ -3391,7 +3391,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3456,7 +3456,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B26">
@@ -3514,7 +3514,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B28">
@@ -3572,7 +3572,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B30">
@@ -3630,7 +3630,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B32">
@@ -3833,7 +3833,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="5" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>